<commit_message>
adding jar for rasp
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\IdeaProjects\RL Tracker3.0\RLTracker3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616139AB-CA6F-42EC-9457-4D0B59398C61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957D8499-FA04-4A17-8451-B9ECAE395168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{3857CAFB-7C99-4F5B-B52D-5D50FBB64C3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3857CAFB-7C99-4F5B-B52D-5D50FBB64C3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -139,7 +142,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.8409300950057299E-2"/>
+          <c:y val="9.2014336917562736E-2"/>
+          <c:w val="0.94085964606536854"/>
+          <c:h val="0.82713041514971919"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -172,51 +185,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$14</c:f>
+              <c:f>Sheet1!$A$1:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
-                  <c:v>1080</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1071</c:v>
+                  <c:v>784</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1080</c:v>
+                  <c:v>797</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1089</c:v>
+                  <c:v>808</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1099</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1108</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1099</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1108</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1117</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1127</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1136</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1145</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1155</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1146</c:v>
+                  <c:v>820</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -399,7 +385,1171 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1068</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1043</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1031</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1042</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1030</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1042</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1054</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1065</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1076</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1087</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1076</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1086</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1096</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1085</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1075</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1085</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1075</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1085</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1095</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1113</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1104</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1113</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1103</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1094</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1131</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1131</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1132</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1132</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1142</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1132</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D41-49E1-8F77-B25386AC89E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="353724047"/>
+        <c:axId val="519115023"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="353724047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="519115023"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="519115023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="353724047"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$A$1:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1071</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1089</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1108</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1108</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1117</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1127</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1136</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1145</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1155</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1137</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1127</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1118</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1108</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1099</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1099</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1091</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1081</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1082</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1091</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0C51-43F8-9E1D-E8B6D203EAB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="649458575"/>
+        <c:axId val="505524559"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="649458575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505524559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="505524559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="649458575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$A$1:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>1163</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1183</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1141</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1161</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1145</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1165</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1186</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1163</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1142</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1164</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1143</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1164</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1147</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1168</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1147</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1124</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1081</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1061</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1081</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1082</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1062</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1018</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1038</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1102</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1081</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1061</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1040</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9910-4C73-BE90-00250EEF9350}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="594106399"/>
+        <c:axId val="514443599"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="594106399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514443599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="514443599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594106399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -942,6 +2092,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -963,6 +3661,129 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5FD7333-65D8-4777-86E3-DA61D46B1ED0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69FA6C9F-1D62-4087-9DA8-00D51452FEAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB8D4C7-B4BF-40D5-8BA5-4B68C017C79A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BDFAE61-941B-47B4-BEDA-91E495D41AC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1282,8 +4103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336C9D72-7423-4092-B831-B140FB98487A}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +4114,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1080</v>
+        <v>771</v>
       </c>
       <c r="B1" s="2">
         <v>44111.924780092595</v>
@@ -1301,7 +4122,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1071</v>
+        <v>784</v>
       </c>
       <c r="B2" s="2">
         <v>44112.029907407406</v>
@@ -1309,7 +4130,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>1080</v>
+        <v>797</v>
       </c>
       <c r="B3" s="2">
         <v>44112.032743055555</v>
@@ -1317,7 +4138,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>1089</v>
+        <v>808</v>
       </c>
       <c r="B4" s="2">
         <v>44112.038425925923</v>
@@ -1325,62 +4146,44 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>1099</v>
+        <v>820</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>1108</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>1099</v>
-      </c>
+      <c r="A7" s="3"/>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>1108</v>
-      </c>
+      <c r="A8" s="3"/>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>1117</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>1127</v>
-      </c>
+      <c r="A10" s="3"/>
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>1136</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>1145</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>1155</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>1146</v>
-      </c>
+      <c r="A14" s="3"/>
       <c r="B14" s="1"/>
     </row>
   </sheetData>
@@ -1388,4 +4191,537 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1186BD6A-D5C3-4E85-B2BC-1632FAC547D6}">
+  <dimension ref="A1:A36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD09E6BB-F114-4112-A974-49E7EB0A1953}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1091</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E84C599-DD4B-4D2C-A5C9-82CA9FB80DD5}">
+  <dimension ref="A1:A34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1040</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>